<commit_message>
adds min/max to metadata and custom units. almost validated, needs project metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/butte_catch_metadata.xlsx
+++ b/data-raw/metadata/butte_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-butte-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC8B454-DA84-D047-B598-5FA8BD0AF7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C13DB1A-D195-734D-82E0-FA5AF1198EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3740" yWindow="-19420" windowWidth="30240" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32060" yWindow="-20740" windowWidth="33720" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -142,9 +142,6 @@
     <t>numeric</t>
   </si>
   <si>
-    <t>millimeters</t>
-  </si>
-  <si>
     <t>real</t>
   </si>
   <si>
@@ -222,11 +219,23 @@
   <si>
     <t>attribute_name</t>
   </si>
+  <si>
+    <t>Butte River RST program</t>
+  </si>
+  <si>
+    <t>millimeter</t>
+  </si>
+  <si>
+    <t>number of fish</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -238,11 +247,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -277,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -302,6 +313,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,9 +531,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -537,7 +549,7 @@
     <col min="9" max="9" width="14.1640625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" customWidth="1"/>
+    <col min="12" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="26" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -597,13 +609,13 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
@@ -673,7 +685,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>25</v>
@@ -685,7 +697,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -799,7 +811,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -837,7 +849,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -875,7 +887,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -913,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -951,7 +963,7 @@
         <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -995,16 +1007,20 @@
         <v>36</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>11273</v>
+      </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -1021,10 +1037,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
@@ -1039,16 +1055,20 @@
         <v>36</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1065,10 +1085,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>36</v>
@@ -1082,15 +1102,21 @@
       <c r="F14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="H14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>88680</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1107,10 +1133,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1119,7 +1145,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1145,10 +1171,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1157,7 +1183,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1183,30 +1209,34 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="6"/>
       <c r="J17" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K17" s="6"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="L17" s="12">
+        <v>42311.413738425923</v>
+      </c>
+      <c r="M17" s="12">
+        <v>44742.416666666664</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -1223,10 +1253,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1235,7 +1265,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1261,10 +1291,10 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>13</v>
@@ -1273,7 +1303,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1299,10 +1329,10 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
@@ -1311,7 +1341,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -28467,8 +28497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28481,13 +28511,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28514,9 +28544,15 @@
       <c r="Z1" s="9"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="A2" s="9">
+        <v>11</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>

</xml_diff>

<commit_message>
updates attributes in butte catch metadata file and adds coverage to overall metadata file. validates
</commit_message>
<xml_diff>
--- a/data-raw/metadata/butte_catch_metadata.xlsx
+++ b/data-raw/metadata/butte_catch_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-butte-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C13DB1A-D195-734D-82E0-FA5AF1198EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F6A472-3793-FA4A-958B-9B2E725B674A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32060" yWindow="-20740" windowWidth="33720" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -100,19 +100,7 @@
     <t>Foreign Key to the CAMP Release table</t>
   </si>
   <si>
-    <t>species</t>
-  </si>
-  <si>
     <t>Common name of species</t>
-  </si>
-  <si>
-    <t>atCaptureRun</t>
-  </si>
-  <si>
-    <t>Run as assigned at the time of the capture.</t>
-  </si>
-  <si>
-    <t>finalRun</t>
   </si>
   <si>
     <t>Run designation as determined in the field or as assigned at a later date. This is the field used in analysis.</t>
@@ -158,9 +146,6 @@
   </si>
   <si>
     <t>whole</t>
-  </si>
-  <si>
-    <t>actualCount</t>
   </si>
   <si>
     <t>Whether the count (n) is an actual count or estimate. Levels = c("Yes", "No")</t>
@@ -228,13 +213,19 @@
   <si>
     <t>number of fish</t>
   </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>actualCountID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -311,9 +302,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,11 +520,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -609,10 +600,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -685,13 +676,13 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
@@ -723,13 +714,13 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -799,7 +790,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
@@ -911,12 +902,12 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
@@ -951,28 +942,38 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>11273</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -989,28 +990,28 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
@@ -1019,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>11273</v>
+        <v>1</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1037,28 +1038,28 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
@@ -1067,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="3">
-        <v>1</v>
+        <v>88680</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1085,38 +1086,28 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="3">
-        <v>0</v>
-      </c>
-      <c r="M14" s="3">
-        <v>88680</v>
-      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1133,28 +1124,34 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="10">
+        <v>42311.413738425923</v>
+      </c>
+      <c r="M15" s="10">
+        <v>44742.416666666664</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1171,10 +1168,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1185,14 +1182,14 @@
       <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1209,54 +1206,48 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5" t="s">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="12">
-        <v>42311.413738425923</v>
-      </c>
-      <c r="M17" s="12">
-        <v>44742.416666666664</v>
-      </c>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-    </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1267,44 +1258,34 @@
       <c r="E18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A19" s="4"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1328,21 +1309,11 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1365,20 +1336,20 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1399,14 +1370,14 @@
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1478,7 +1449,7 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
@@ -1506,19 +1477,6 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -1534,11 +1492,6 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1562,75 +1515,36 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -1646,19 +1560,6 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1786,7 +1687,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1814,7 +1715,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1842,7 +1743,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1870,7 +1771,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -2542,7 +2443,7 @@
       <c r="Z62" s="1"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
+      <c r="A63" s="4"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="2"/>
@@ -2570,7 +2471,7 @@
       <c r="Z63" s="1"/>
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
+      <c r="A64" s="4"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="2"/>
@@ -2598,7 +2499,7 @@
       <c r="Z64" s="1"/>
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1"/>
+      <c r="A65" s="4"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="2"/>
@@ -2626,7 +2527,7 @@
       <c r="Z65" s="1"/>
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1"/>
+      <c r="A66" s="4"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="2"/>
@@ -2654,7 +2555,7 @@
       <c r="Z66" s="1"/>
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1"/>
+      <c r="A67" s="4"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="2"/>
@@ -2682,7 +2583,7 @@
       <c r="Z67" s="1"/>
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1"/>
+      <c r="A68" s="4"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="2"/>
@@ -2710,7 +2611,7 @@
       <c r="Z68" s="1"/>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1"/>
+      <c r="A69" s="4"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="2"/>
@@ -2738,7 +2639,7 @@
       <c r="Z69" s="1"/>
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
+      <c r="A70" s="4"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="2"/>
@@ -2766,7 +2667,7 @@
       <c r="Z70" s="1"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
+      <c r="A71" s="4"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="2"/>
@@ -2794,7 +2695,7 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
+      <c r="A72" s="4"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
@@ -2822,7 +2723,7 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="2"/>
@@ -28469,22 +28370,330 @@
       <c r="Y988" s="1"/>
       <c r="Z988" s="1"/>
     </row>
+    <row r="989" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A989" s="1"/>
+      <c r="B989" s="1"/>
+      <c r="C989" s="1"/>
+      <c r="D989" s="2"/>
+      <c r="E989" s="1"/>
+      <c r="F989" s="3"/>
+      <c r="G989" s="3"/>
+      <c r="H989" s="3"/>
+      <c r="I989" s="2"/>
+      <c r="J989" s="3"/>
+      <c r="K989" s="2"/>
+      <c r="L989" s="3"/>
+      <c r="M989" s="3"/>
+      <c r="N989" s="1"/>
+      <c r="O989" s="1"/>
+      <c r="P989" s="1"/>
+      <c r="Q989" s="1"/>
+      <c r="R989" s="1"/>
+      <c r="S989" s="1"/>
+      <c r="T989" s="1"/>
+      <c r="U989" s="1"/>
+      <c r="V989" s="1"/>
+      <c r="W989" s="1"/>
+      <c r="X989" s="1"/>
+      <c r="Y989" s="1"/>
+      <c r="Z989" s="1"/>
+    </row>
+    <row r="990" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A990" s="1"/>
+      <c r="B990" s="1"/>
+      <c r="C990" s="1"/>
+      <c r="D990" s="2"/>
+      <c r="E990" s="1"/>
+      <c r="F990" s="3"/>
+      <c r="G990" s="3"/>
+      <c r="H990" s="3"/>
+      <c r="I990" s="2"/>
+      <c r="J990" s="3"/>
+      <c r="K990" s="2"/>
+      <c r="L990" s="3"/>
+      <c r="M990" s="3"/>
+      <c r="N990" s="1"/>
+      <c r="O990" s="1"/>
+      <c r="P990" s="1"/>
+      <c r="Q990" s="1"/>
+      <c r="R990" s="1"/>
+      <c r="S990" s="1"/>
+      <c r="T990" s="1"/>
+      <c r="U990" s="1"/>
+      <c r="V990" s="1"/>
+      <c r="W990" s="1"/>
+      <c r="X990" s="1"/>
+      <c r="Y990" s="1"/>
+      <c r="Z990" s="1"/>
+    </row>
+    <row r="991" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A991" s="1"/>
+      <c r="B991" s="1"/>
+      <c r="C991" s="1"/>
+      <c r="D991" s="2"/>
+      <c r="E991" s="1"/>
+      <c r="F991" s="3"/>
+      <c r="G991" s="3"/>
+      <c r="H991" s="3"/>
+      <c r="I991" s="2"/>
+      <c r="J991" s="3"/>
+      <c r="K991" s="2"/>
+      <c r="L991" s="3"/>
+      <c r="M991" s="3"/>
+      <c r="N991" s="1"/>
+      <c r="O991" s="1"/>
+      <c r="P991" s="1"/>
+      <c r="Q991" s="1"/>
+      <c r="R991" s="1"/>
+      <c r="S991" s="1"/>
+      <c r="T991" s="1"/>
+      <c r="U991" s="1"/>
+      <c r="V991" s="1"/>
+      <c r="W991" s="1"/>
+      <c r="X991" s="1"/>
+      <c r="Y991" s="1"/>
+      <c r="Z991" s="1"/>
+    </row>
+    <row r="992" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A992" s="1"/>
+      <c r="B992" s="1"/>
+      <c r="C992" s="1"/>
+      <c r="D992" s="2"/>
+      <c r="E992" s="1"/>
+      <c r="F992" s="3"/>
+      <c r="G992" s="3"/>
+      <c r="H992" s="3"/>
+      <c r="I992" s="2"/>
+      <c r="J992" s="3"/>
+      <c r="K992" s="2"/>
+      <c r="L992" s="3"/>
+      <c r="M992" s="3"/>
+      <c r="N992" s="1"/>
+      <c r="O992" s="1"/>
+      <c r="P992" s="1"/>
+      <c r="Q992" s="1"/>
+      <c r="R992" s="1"/>
+      <c r="S992" s="1"/>
+      <c r="T992" s="1"/>
+      <c r="U992" s="1"/>
+      <c r="V992" s="1"/>
+      <c r="W992" s="1"/>
+      <c r="X992" s="1"/>
+      <c r="Y992" s="1"/>
+      <c r="Z992" s="1"/>
+    </row>
+    <row r="993" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A993" s="1"/>
+      <c r="B993" s="1"/>
+      <c r="C993" s="1"/>
+      <c r="D993" s="2"/>
+      <c r="E993" s="1"/>
+      <c r="F993" s="3"/>
+      <c r="G993" s="3"/>
+      <c r="H993" s="3"/>
+      <c r="I993" s="2"/>
+      <c r="J993" s="3"/>
+      <c r="K993" s="2"/>
+      <c r="L993" s="3"/>
+      <c r="M993" s="3"/>
+      <c r="N993" s="1"/>
+      <c r="O993" s="1"/>
+      <c r="P993" s="1"/>
+      <c r="Q993" s="1"/>
+      <c r="R993" s="1"/>
+      <c r="S993" s="1"/>
+      <c r="T993" s="1"/>
+      <c r="U993" s="1"/>
+      <c r="V993" s="1"/>
+      <c r="W993" s="1"/>
+      <c r="X993" s="1"/>
+      <c r="Y993" s="1"/>
+      <c r="Z993" s="1"/>
+    </row>
+    <row r="994" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A994" s="1"/>
+      <c r="B994" s="1"/>
+      <c r="C994" s="1"/>
+      <c r="D994" s="2"/>
+      <c r="E994" s="1"/>
+      <c r="F994" s="3"/>
+      <c r="G994" s="3"/>
+      <c r="H994" s="3"/>
+      <c r="I994" s="2"/>
+      <c r="J994" s="3"/>
+      <c r="K994" s="2"/>
+      <c r="L994" s="3"/>
+      <c r="M994" s="3"/>
+      <c r="N994" s="1"/>
+      <c r="O994" s="1"/>
+      <c r="P994" s="1"/>
+      <c r="Q994" s="1"/>
+      <c r="R994" s="1"/>
+      <c r="S994" s="1"/>
+      <c r="T994" s="1"/>
+      <c r="U994" s="1"/>
+      <c r="V994" s="1"/>
+      <c r="W994" s="1"/>
+      <c r="X994" s="1"/>
+      <c r="Y994" s="1"/>
+      <c r="Z994" s="1"/>
+    </row>
+    <row r="995" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A995" s="1"/>
+      <c r="B995" s="1"/>
+      <c r="C995" s="1"/>
+      <c r="D995" s="2"/>
+      <c r="E995" s="1"/>
+      <c r="F995" s="3"/>
+      <c r="G995" s="3"/>
+      <c r="H995" s="3"/>
+      <c r="I995" s="2"/>
+      <c r="J995" s="3"/>
+      <c r="K995" s="2"/>
+      <c r="L995" s="3"/>
+      <c r="M995" s="3"/>
+      <c r="N995" s="1"/>
+      <c r="O995" s="1"/>
+      <c r="P995" s="1"/>
+      <c r="Q995" s="1"/>
+      <c r="R995" s="1"/>
+      <c r="S995" s="1"/>
+      <c r="T995" s="1"/>
+      <c r="U995" s="1"/>
+      <c r="V995" s="1"/>
+      <c r="W995" s="1"/>
+      <c r="X995" s="1"/>
+      <c r="Y995" s="1"/>
+      <c r="Z995" s="1"/>
+    </row>
+    <row r="996" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A996" s="1"/>
+      <c r="B996" s="1"/>
+      <c r="C996" s="1"/>
+      <c r="D996" s="2"/>
+      <c r="E996" s="1"/>
+      <c r="F996" s="3"/>
+      <c r="G996" s="3"/>
+      <c r="H996" s="3"/>
+      <c r="I996" s="2"/>
+      <c r="J996" s="3"/>
+      <c r="K996" s="2"/>
+      <c r="L996" s="3"/>
+      <c r="M996" s="3"/>
+      <c r="N996" s="1"/>
+      <c r="O996" s="1"/>
+      <c r="P996" s="1"/>
+      <c r="Q996" s="1"/>
+      <c r="R996" s="1"/>
+      <c r="S996" s="1"/>
+      <c r="T996" s="1"/>
+      <c r="U996" s="1"/>
+      <c r="V996" s="1"/>
+      <c r="W996" s="1"/>
+      <c r="X996" s="1"/>
+      <c r="Y996" s="1"/>
+      <c r="Z996" s="1"/>
+    </row>
+    <row r="997" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A997" s="1"/>
+      <c r="B997" s="1"/>
+      <c r="C997" s="1"/>
+      <c r="D997" s="2"/>
+      <c r="E997" s="1"/>
+      <c r="F997" s="3"/>
+      <c r="G997" s="3"/>
+      <c r="H997" s="3"/>
+      <c r="I997" s="2"/>
+      <c r="J997" s="3"/>
+      <c r="K997" s="2"/>
+      <c r="L997" s="3"/>
+      <c r="M997" s="3"/>
+      <c r="N997" s="1"/>
+      <c r="O997" s="1"/>
+      <c r="P997" s="1"/>
+      <c r="Q997" s="1"/>
+      <c r="R997" s="1"/>
+      <c r="S997" s="1"/>
+      <c r="T997" s="1"/>
+      <c r="U997" s="1"/>
+      <c r="V997" s="1"/>
+      <c r="W997" s="1"/>
+      <c r="X997" s="1"/>
+      <c r="Y997" s="1"/>
+      <c r="Z997" s="1"/>
+    </row>
+    <row r="998" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A998" s="1"/>
+      <c r="B998" s="1"/>
+      <c r="C998" s="1"/>
+      <c r="D998" s="2"/>
+      <c r="E998" s="1"/>
+      <c r="F998" s="3"/>
+      <c r="G998" s="3"/>
+      <c r="H998" s="3"/>
+      <c r="I998" s="2"/>
+      <c r="J998" s="3"/>
+      <c r="K998" s="2"/>
+      <c r="L998" s="3"/>
+      <c r="M998" s="3"/>
+      <c r="N998" s="1"/>
+      <c r="O998" s="1"/>
+      <c r="P998" s="1"/>
+      <c r="Q998" s="1"/>
+      <c r="R998" s="1"/>
+      <c r="S998" s="1"/>
+      <c r="T998" s="1"/>
+      <c r="U998" s="1"/>
+      <c r="V998" s="1"/>
+      <c r="W998" s="1"/>
+      <c r="X998" s="1"/>
+      <c r="Y998" s="1"/>
+      <c r="Z998" s="1"/>
+    </row>
+    <row r="999" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A999" s="1"/>
+      <c r="B999" s="1"/>
+      <c r="C999" s="1"/>
+      <c r="D999" s="2"/>
+      <c r="E999" s="1"/>
+      <c r="F999" s="3"/>
+      <c r="G999" s="3"/>
+      <c r="H999" s="3"/>
+      <c r="I999" s="2"/>
+      <c r="J999" s="3"/>
+      <c r="K999" s="2"/>
+      <c r="L999" s="3"/>
+      <c r="M999" s="3"/>
+      <c r="N999" s="1"/>
+      <c r="O999" s="1"/>
+      <c r="P999" s="1"/>
+      <c r="Q999" s="1"/>
+      <c r="R999" s="1"/>
+      <c r="S999" s="1"/>
+      <c r="T999" s="1"/>
+      <c r="U999" s="1"/>
+      <c r="V999" s="1"/>
+      <c r="W999" s="1"/>
+      <c r="X999" s="1"/>
+      <c r="Y999" s="1"/>
+      <c r="Z999" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E988" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C56:C999 C32:C44 C1:C25" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E32:E999 E1:E25" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F988" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F27 F32:F999 F1:F25" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C33 C45:C988" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H988" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H27 H32:H999 H1:H25" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28511,13 +28720,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28548,10 +28757,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>

</xml_diff>

<commit_message>
reads in correct data sheets and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/butte_catch_metadata.xlsx
+++ b/data-raw/metadata/butte_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-butte-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F6A472-3793-FA4A-958B-9B2E725B674A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5C5DCA-9D41-1B47-916F-1BF21006F06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32060" yWindow="-20740" windowWidth="33720" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9440" yWindow="-21600" windowWidth="19040" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -151,12 +151,6 @@
     <t>Whether the count (n) is an actual count or estimate. Levels = c("Yes", "No")</t>
   </si>
   <si>
-    <t>mort</t>
-  </si>
-  <si>
-    <t>Whether fish died due to being captured or handled.  Levels = c("Yes", "No")</t>
-  </si>
-  <si>
     <t>visitTime</t>
   </si>
   <si>
@@ -214,10 +208,16 @@
     <t>number of fish</t>
   </si>
   <si>
-    <t>run</t>
+    <t>atCaptureRun</t>
   </si>
   <si>
-    <t>actualCountID</t>
+    <t>finalRun</t>
+  </si>
+  <si>
+    <t>actualCount</t>
+  </si>
+  <si>
+    <t>Run designation revised after field visit.</t>
   </si>
 </sst>
 </file>
@@ -520,11 +520,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -600,10 +600,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -714,7 +714,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
@@ -904,28 +904,38 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>11273</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -942,10 +952,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -960,7 +970,7 @@
         <v>32</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>34</v>
@@ -972,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="3">
-        <v>11273</v>
+        <v>590</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -990,10 +1000,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1008,10 +1018,10 @@
         <v>32</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
@@ -1020,7 +1030,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>1</v>
+        <v>88680</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1038,37 +1048,33 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>32</v>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="5" t="s">
+        <v>44</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>61</v>
+      <c r="K13" s="6"/>
+      <c r="L13" s="10">
+        <v>42311.413738425923</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="3">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3">
-        <v>88680</v>
+      <c r="M13" s="10">
+        <v>44742.417013888888</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1086,10 +1092,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1100,14 +1106,14 @@
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1124,34 +1130,28 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="10">
-        <v>42311.413738425923</v>
-      </c>
-      <c r="M15" s="10">
-        <v>44742.416666666664</v>
-      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1182,14 +1182,14 @@
       <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1206,10 +1206,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1244,10 +1244,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1308,20 +1308,20 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1336,7 +1336,7 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1348,8 +1348,8 @@
       <c r="I21" s="6"/>
       <c r="J21" s="5"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1370,14 +1370,14 @@
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1449,19 +1449,6 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1477,6 +1464,14 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -1492,27 +1487,19 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N28" s="4"/>
@@ -1530,19 +1517,19 @@
       <c r="Z28" s="4"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N30" s="1"/>
@@ -1560,6 +1547,19 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1659,7 +1659,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -1687,7 +1687,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1715,7 +1715,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="12"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1743,7 +1743,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1771,7 +1771,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -2723,7 +2723,7 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="4"/>
+      <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="2"/>
@@ -28650,50 +28650,22 @@
       <c r="Y998" s="1"/>
       <c r="Z998" s="1"/>
     </row>
-    <row r="999" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A999" s="1"/>
-      <c r="B999" s="1"/>
-      <c r="C999" s="1"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="1"/>
-      <c r="F999" s="3"/>
-      <c r="G999" s="3"/>
-      <c r="H999" s="3"/>
-      <c r="I999" s="2"/>
-      <c r="J999" s="3"/>
-      <c r="K999" s="2"/>
-      <c r="L999" s="3"/>
-      <c r="M999" s="3"/>
-      <c r="N999" s="1"/>
-      <c r="O999" s="1"/>
-      <c r="P999" s="1"/>
-      <c r="Q999" s="1"/>
-      <c r="R999" s="1"/>
-      <c r="S999" s="1"/>
-      <c r="T999" s="1"/>
-      <c r="U999" s="1"/>
-      <c r="V999" s="1"/>
-      <c r="W999" s="1"/>
-      <c r="X999" s="1"/>
-      <c r="Y999" s="1"/>
-      <c r="Z999" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C56:C999 C32:C44 C1:C25" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C55:C998 C31:C43 C1:C24" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E32:E999 E1:E25" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E31:E998 E1:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F27 F32:F999 F1:F25" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F26 F31:F998 F1:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H27 H32:H999 H1:H25" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H26 H31:H998 H1:H24" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28720,13 +28692,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28757,10 +28729,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>

</xml_diff>

<commit_message>
fixes code definition tab and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/butte_catch_metadata.xlsx
+++ b/data-raw/metadata/butte_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-butte-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5C5DCA-9D41-1B47-916F-1BF21006F06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDC59EC-D0C4-7D46-B271-A2BD72941E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9440" yWindow="-21600" windowWidth="19040" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9440" yWindow="-21100" windowWidth="19040" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>attribute_name</t>
   </si>
   <si>
-    <t>Butte River RST program</t>
-  </si>
-  <si>
     <t>millimeter</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>Run designation revised after field visit.</t>
+  </si>
+  <si>
+    <t>Butte Creek RST program</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
     </sheetView>
@@ -790,7 +790,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
@@ -922,7 +922,7 @@
         <v>32</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>34</v>
@@ -970,7 +970,7 @@
         <v>32</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>34</v>
@@ -1018,7 +1018,7 @@
         <v>32</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>39</v>
@@ -1206,10 +1206,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>40</v>
@@ -28678,8 +28678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28729,7 +28729,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
updates metadata tables to reflect new files from grant
</commit_message>
<xml_diff>
--- a/data-raw/metadata/butte_catch_metadata.xlsx
+++ b/data-raw/metadata/butte_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-butte-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDC59EC-D0C4-7D46-B271-A2BD72941E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B81C30A-990B-064A-9521-3804307D1D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9440" yWindow="-21100" windowWidth="19040" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="760" windowWidth="16740" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -172,13 +172,7 @@
     <t>siteName</t>
   </si>
   <si>
-    <t>Name of the sampling site. Levels = c("Parrott-Phelan canal trap box", "Okie RST", "Parrott-Phelan RST")</t>
-  </si>
-  <si>
     <t>subSiteName</t>
-  </si>
-  <si>
-    <t>Name of the trap or trap location. Levels = c("canal trap box", "Okie RST", "PP RST")</t>
   </si>
   <si>
     <t>ProjectDescriptionID</t>
@@ -218,6 +212,13 @@
   </si>
   <si>
     <t>Butte Creek RST program</t>
+  </si>
+  <si>
+    <t>Name of the sampling site. Levels = c("Parrott-Phelan canal trap box", "Parrot-Phelan RST", "Coleman National Fish Hatchery"
+)</t>
+  </si>
+  <si>
+    <t>Name of the trap or trap location. Levels = c("canal trap box", "PP RST", "n/a")</t>
   </si>
 </sst>
 </file>
@@ -522,9 +523,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -600,10 +601,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -714,7 +715,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
@@ -790,7 +791,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
@@ -922,7 +923,7 @@
         <v>32</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>34</v>
@@ -934,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="3">
-        <v>11273</v>
+        <v>1000</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -970,7 +971,7 @@
         <v>32</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>34</v>
@@ -1018,7 +1019,7 @@
         <v>32</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>39</v>
@@ -1074,7 +1075,7 @@
         <v>42311.413738425923</v>
       </c>
       <c r="M13" s="10">
-        <v>44742.417013888888</v>
+        <v>44929.489618055559</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1133,7 +1134,7 @@
         <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1168,10 +1169,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1206,10 +1207,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1244,7 +1245,7 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>40</v>
@@ -28678,7 +28679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -28692,13 +28693,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28729,10 +28730,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>

</xml_diff>

<commit_message>
updates descriptions in metadata attributes. updates personnel in project metadata and license
</commit_message>
<xml_diff>
--- a/data-raw/metadata/butte_catch_metadata.xlsx
+++ b/data-raw/metadata/butte_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-butte-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B81C30A-990B-064A-9521-3804307D1D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8804E080-BA3C-EF49-B6A6-B3255FA1FB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="760" windowWidth="16740" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -100,12 +100,6 @@
     <t>Foreign Key to the CAMP Release table</t>
   </si>
   <si>
-    <t>Common name of species</t>
-  </si>
-  <si>
-    <t>Run designation as determined in the field or as assigned at a later date. This is the field used in analysis.</t>
-  </si>
-  <si>
     <t>fishOrigin</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
   </si>
   <si>
     <t>lifeStage</t>
-  </si>
-  <si>
-    <t>Life stage of the fish. Levels = c("Not recorded", "Smolt", "Parr", "Fry", "Button-up fry", "Silvery parr", "Adult", "Juvenile", "Ammocoete", "Yearling", "Yolk sac fry (alevin)")</t>
   </si>
   <si>
     <t>forkLength</t>
@@ -166,9 +157,6 @@
     <t>visitType</t>
   </si>
   <si>
-    <t>Work that was done during visit to trap. Levels = c("Continue trapping", "Start trap &amp; begin trapping", "End trapping", "Unplanned restart", "Not applicable (n/a)", "Service/adjust/clean trap")</t>
-  </si>
-  <si>
     <t>siteName</t>
   </si>
   <si>
@@ -208,17 +196,40 @@
     <t>actualCount</t>
   </si>
   <si>
-    <t>Run designation revised after field visit.</t>
-  </si>
-  <si>
     <t>Butte Creek RST program</t>
   </si>
   <si>
+    <t>Name of the trap or trap location. Levels = c("canal trap box", "PP RST", "n/a")</t>
+  </si>
+  <si>
+    <t>Common name of species. Levels = c("Chinook salmon", "Steelhead / rainbow trout", "Hardhead", 
+"Riffle sculpin", "Sacramento pikeminnow", "Sacramento sucker", 
+"California roach", "Pacific lamprey", "Tule perch", "Green sunfish", 
+"Unknown lamprey (Entosphenus or Lampetra)", "Brown trout", "Redear sunfish", 
+"Bluegill", "Brown bullhead", "Other", "Unknown minnow", "Largemouth bass", 
+"River lamprey", "Unknown crappie (Pomoxis)", "Smallmouth bass", 
+"Pacific lamprey (no longer valid)", "Western brook lamprey", 
+"Unknown Centrarchid")</t>
+  </si>
+  <si>
+    <t>Run designation as determined in the field or as assigned at a later date. This is the field used in analysis. Levels = c("Not recorded", "Spring", "Fall", "Winter").</t>
+  </si>
+  <si>
+    <t>Life stage of the fish. Levels = c("Not recorded", "Smolt", "Parr", "Fry", "Button-up fry", "Silvery parr", 
+"Juvenile", "Ammocoete", "Yearling", "Yolk sac fry (alevin)")</t>
+  </si>
+  <si>
+    <t>Work that was done during visit to trap. Levels = c("Continue trapping", "Start trap &amp; begin trapping", "End trapping", 
+"Unplanned restart", "Not applicable (n/a)", "Service/adjust/clean trap", 
+NA)</t>
+  </si>
+  <si>
     <t>Name of the sampling site. Levels = c("Parrott-Phelan canal trap box", "Parrot-Phelan RST", "Coleman National Fish Hatchery"
+)
 )</t>
   </si>
   <si>
-    <t>Name of the trap or trap location. Levels = c("canal trap box", "PP RST", "n/a")</t>
+    <t>Run designation revised after field visit. Levels = c(NA, "Not recorded", "Fall", "Spring", "Winter").</t>
   </si>
 </sst>
 </file>
@@ -525,7 +536,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -601,10 +612,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -715,10 +726,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -791,10 +802,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -829,10 +840,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -867,10 +878,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -905,28 +916,28 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
@@ -953,28 +964,28 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
@@ -1001,28 +1012,28 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
@@ -1049,26 +1060,26 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
       <c r="J13" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="10">
@@ -1093,10 +1104,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1131,7 +1142,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>62</v>
@@ -1169,10 +1180,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1207,10 +1218,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1245,10 +1256,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -28693,13 +28704,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28730,10 +28741,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>

</xml_diff>

<commit_message>
adds historical catch from cloud to catch for butte. updates metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/butte_catch_metadata.xlsx
+++ b/data-raw/metadata/butte_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-butte-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8804E080-BA3C-EF49-B6A6-B3255FA1FB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A29049E-90F8-2E47-A62E-60C2A4EDB4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -166,9 +166,6 @@
     <t>ProjectDescriptionID</t>
   </si>
   <si>
-    <t>Foreign key to the CAMP ProjectDescription table. All data associated with this package will have a ProjectDescriptionID = 11</t>
-  </si>
-  <si>
     <t>commonName</t>
   </si>
   <si>
@@ -199,37 +196,41 @@
     <t>Butte Creek RST program</t>
   </si>
   <si>
-    <t>Name of the trap or trap location. Levels = c("canal trap box", "PP RST", "n/a")</t>
-  </si>
-  <si>
-    <t>Common name of species. Levels = c("Chinook salmon", "Steelhead / rainbow trout", "Hardhead", 
-"Riffle sculpin", "Sacramento pikeminnow", "Sacramento sucker", 
-"California roach", "Pacific lamprey", "Tule perch", "Green sunfish", 
-"Unknown lamprey (Entosphenus or Lampetra)", "Brown trout", "Redear sunfish", 
-"Bluegill", "Brown bullhead", "Other", "Unknown minnow", "Largemouth bass", 
-"River lamprey", "Unknown crappie (Pomoxis)", "Smallmouth bass", 
-"Pacific lamprey (no longer valid)", "Western brook lamprey", 
-"Unknown Centrarchid")</t>
-  </si>
-  <si>
-    <t>Run designation as determined in the field or as assigned at a later date. This is the field used in analysis. Levels = c("Not recorded", "Spring", "Fall", "Winter").</t>
-  </si>
-  <si>
-    <t>Life stage of the fish. Levels = c("Not recorded", "Smolt", "Parr", "Fry", "Button-up fry", "Silvery parr", 
-"Juvenile", "Ammocoete", "Yearling", "Yolk sac fry (alevin)")</t>
-  </si>
-  <si>
     <t>Work that was done during visit to trap. Levels = c("Continue trapping", "Start trap &amp; begin trapping", "End trapping", 
 "Unplanned restart", "Not applicable (n/a)", "Service/adjust/clean trap", 
 NA)</t>
   </si>
   <si>
-    <t>Name of the sampling site. Levels = c("Parrott-Phelan canal trap box", "Parrot-Phelan RST", "Coleman National Fish Hatchery"
-)
-)</t>
+    <t>Run designation revised after field visit. Levels = c(NA, "Not recorded", "Fall", "Spring", "Winter").</t>
   </si>
   <si>
-    <t>Run designation revised after field visit. Levels = c(NA, "Not recorded", "Fall", "Spring", "Winter").</t>
+    <t>Foreign key to the CAMP ProjectDescription table. All CAMP data associated with this package will have a ProjectDescriptionID = 11</t>
+  </si>
+  <si>
+    <t>Common name of species. Levels = c("chinook salmon", "steelhead / rainbow trout", "hardhead", 
+"riffle sculpin", "sacramento pikeminnow", "sacramento sucker", 
+"california roach", "pacific lamprey", "tule perch", "green sunfish", 
+"unknown lamprey (entosphenus or lampetra)", "brown trout", "redear sunfish", 
+"bluegill", "brown bullhead", "other", "unknown minnow", "largemouth bass", 
+"river lamprey", "unknown crappie (pomoxis)", "smallmouth bass", 
+"pacific lamprey (no longer valid)", "western brook lamprey", 
+"unknown centrarchid")</t>
+  </si>
+  <si>
+    <t>Run designation as determined in the field or as assigned at a later date. This is the field used in analysis. Levels = c("not recorded", "spring", "fall", "winter").</t>
+  </si>
+  <si>
+    <t>Life stage of the fish. Levels = c("not recorded", "smolt", "parr", "fry", "button-up fry", "silvery parr", 
+"juvenile", "ammocoete", "yearling", "yolk sac fry (alevin)", 
+"adult", "yolk sac fry", "unknown", NA)</t>
+  </si>
+  <si>
+    <t>Name of the sampling site. Levels = c("parrott-phelan canal trap box", "parrot-phelan rst", "coleman national fish hatchery", 
+"okie dam", "adams dam")</t>
+  </si>
+  <si>
+    <t>Name of the trap or trap location. Levels = c("canal trap box", "pp rst", "n/a", "okie dam 1", "okie dam fyke trap", 
+NA, "adams dam", "okie dam 2")</t>
   </si>
 </sst>
 </file>
@@ -536,7 +537,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -615,7 +616,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -726,10 +727,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -802,10 +803,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -881,7 +882,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -934,7 +935,7 @@
         <v>29</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>31</v>
@@ -946,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="3">
-        <v>1000</v>
+        <v>1786</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -982,7 +983,7 @@
         <v>29</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>31</v>
@@ -1030,7 +1031,7 @@
         <v>29</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>36</v>
@@ -1042,7 +1043,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>88680</v>
+        <v>220000</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1083,7 +1084,7 @@
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="10">
-        <v>42311.413738425923</v>
+        <v>35034</v>
       </c>
       <c r="M13" s="10">
         <v>44929.489618055559</v>
@@ -1107,7 +1108,7 @@
         <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1183,7 +1184,7 @@
         <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1218,10 +1219,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1256,7 +1257,7 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>37</v>
@@ -28704,13 +28705,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28741,7 +28742,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
adds in trap historical data and updates metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/butte_catch_metadata.xlsx
+++ b/data-raw/metadata/butte_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-butte-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A29049E-90F8-2E47-A62E-60C2A4EDB4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB2730D-0DCB-DD4B-8156-80B3ECED6F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -225,12 +225,10 @@
 "adult", "yolk sac fry", "unknown", NA)</t>
   </si>
   <si>
-    <t>Name of the sampling site. Levels = c("parrott-phelan canal trap box", "parrot-phelan rst", "coleman national fish hatchery", 
-"okie dam", "adams dam")</t>
+    <t>Name of the sampling site. Levels = c("parrot-phelan", "coleman national fish hatchery", "adams dam")</t>
   </si>
   <si>
-    <t>Name of the trap or trap location. Levels = c("canal trap box", "pp rst", "n/a", "okie dam 1", "okie dam fyke trap", 
-NA, "adams dam", "okie dam 2")</t>
+    <t>Name of the trap or trap location. Levels = c("canal trap box", "pp rst", "n/a", NA, "adams dam", "pp rst 2")</t>
   </si>
 </sst>
 </file>

</xml_diff>